<commit_message>
Logica para envio de mensagens com o texto acoplado ao documento
</commit_message>
<xml_diff>
--- a/QRsend1366/src/dados.xlsx
+++ b/QRsend1366/src/dados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,10 +436,18 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>11 964440570</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>11 983787869</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>